<commit_message>
attempt to reduce error rate
</commit_message>
<xml_diff>
--- a/vaccine_data.xlsx
+++ b/vaccine_data.xlsx
@@ -1,78 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epivo/Documents/vaccine_project/vaccine_track/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6A2EF1-AA4A-BC4D-B846-7B1738DD972D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="7260" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Total Doses Distributed</t>
-  </si>
-  <si>
-    <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
-  </si>
-  <si>
-    <t>Doses Distributed for Use in Long-Term Care Facilities</t>
-  </si>
-  <si>
-    <t>Number of People Initiating Vaccination (1st Dose Received) in Long-Term Care Facilities</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,18 +50,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -106,25 +61,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,186 +426,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Doses Distributed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Doses Distributed for Use in Long-Term Care Facilities</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Number of People Initiating Vaccination (1st Dose Received) in Long-Term Care Facilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>44178</v>
+      </c>
+      <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>44178</v>
-      </c>
-      <c r="B2">
+      <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>44195</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>12409050</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>2589125</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>2166200</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>167149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>44198</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>13071925</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>4225756</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>2217025</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>282740</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>44201</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>17020575</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>4836469</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>3260775</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>429066</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>44202</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>17288950</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>5306797</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>3416875</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>511635</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>44203</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>21419800</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>5919418</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>3770425</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>603313</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>44204</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>22137350</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>6688231</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>4060225</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>693246</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>44207</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>25480725</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>8987322</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>4239775</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>937028</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>44208</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>27696150</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>9327138</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>4385175</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>951774</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B11" t="n">
+        <v>29380125</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10278462</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4556575</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1084177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CDC changed time tag and update frq
</commit_message>
<xml_diff>
--- a/vaccine_data.xlsx
+++ b/vaccine_data.xlsx
@@ -1,41 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epivo/Documents/vaccine_project/vaccine_track/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EA84E9-F77F-804D-9AEF-4AA11DF31A71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="5100" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Total Doses Distributed</t>
+  </si>
+  <si>
+    <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
+  </si>
+  <si>
+    <t>Doses Distributed for Use in Long-Term Care Facilities</t>
+  </si>
+  <si>
+    <t>Total Doses Administered</t>
+  </si>
+  <si>
+    <t>Number of People Receiving 1 or More Doses</t>
+  </si>
+  <si>
+    <t>Number of People Receiving 2 Doses</t>
+  </si>
+  <si>
+    <t>Doses Administered in Long-Term Care Facilities</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,10 +95,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -61,84 +114,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,214 +420,333 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total Doses Distributed</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Doses Distributed for Use in Long-Term Care Facilities</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Number of People Initiating Vaccination (1st Dose Received) in Long-Term Care Facilities</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>44178</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>44195</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>12409050</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>2589125</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2166200</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
+        <v>2589125</v>
+      </c>
+      <c r="F3">
+        <v>2589125</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>167149</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>44198</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>13071925</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>4225756</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>2217025</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
+        <v>4225756</v>
+      </c>
+      <c r="F4">
+        <v>4225756</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>282740</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>44201</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>17020575</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>4836469</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>3260775</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
+        <v>4836469</v>
+      </c>
+      <c r="F5">
+        <v>4836469</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>429066</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>44202</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>17288950</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>5306797</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>3416875</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
+        <v>5306797</v>
+      </c>
+      <c r="F6">
+        <v>5306797</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>511635</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>44203</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>21419800</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>5919418</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>3770425</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
+        <v>5919418</v>
+      </c>
+      <c r="F7">
+        <v>5919418</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>603313</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>44204</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>22137350</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>6688231</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>4060225</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
+        <v>6688231</v>
+      </c>
+      <c r="F8">
+        <v>6688231</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>693246</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>44207</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>25480725</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>8987322</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>4239775</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
+        <v>8987322</v>
+      </c>
+      <c r="F9">
+        <v>8987322</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>937028</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>44208</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>27696150</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>9327138</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>4385175</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
+        <v>9327138</v>
+      </c>
+      <c r="F10">
+        <v>9327138</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>951774</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>44209</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>29380125</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>10278462</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>4556575</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
+        <v>10278462</v>
+      </c>
+      <c r="F11">
+        <v>10278462</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>1084177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B12">
+        <v>30628175</v>
+      </c>
+      <c r="C12">
+        <f>F12-G12</f>
+        <v>8348671</v>
+      </c>
+      <c r="E12">
+        <v>11148991</v>
+      </c>
+      <c r="F12">
+        <v>9690757</v>
+      </c>
+      <c r="G12">
+        <v>1342086</v>
+      </c>
+      <c r="H12">
+        <v>1225493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change update time to 7pm
</commit_message>
<xml_diff>
--- a/vaccine_data.xlsx
+++ b/vaccine_data.xlsx
@@ -1,86 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epivo/Documents/vaccine_project/vaccine_track/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EA84E9-F77F-804D-9AEF-4AA11DF31A71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Total Doses Distributed</t>
-  </si>
-  <si>
-    <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
-  </si>
-  <si>
-    <t>Doses Distributed for Use in Long-Term Care Facilities</t>
-  </si>
-  <si>
-    <t>Total Doses Administered</t>
-  </si>
-  <si>
-    <t>Number of People Receiving 1 or More Doses</t>
-  </si>
-  <si>
-    <t>Number of People Receiving 2 Doses</t>
-  </si>
-  <si>
-    <t>Doses Administered in Long-Term Care Facilities</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,18 +50,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -114,25 +61,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,333 +426,387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Doses Distributed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of People Initiating Vaccination (1st Dose Received)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Doses Distributed for Use in Long-Term Care Facilities</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Doses Administered</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Number of People Receiving 1 or More Doses</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Number of People Receiving 2 Doses</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doses Administered in Long-Term Care Facilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>44178</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>44195</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>12409050</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>2589125</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>2166200</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>2589125</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>2589125</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>167149</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>44198</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>13071925</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>4225756</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>2217025</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>4225756</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>4225756</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>282740</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>44201</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>17020575</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>4836469</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>3260775</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>4836469</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>4836469</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>429066</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>44202</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>17288950</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>5306797</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>3416875</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>5306797</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>5306797</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>511635</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>44203</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>21419800</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>5919418</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>3770425</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>5919418</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>5919418</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>603313</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>44204</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>22137350</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>6688231</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>4060225</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>6688231</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>6688231</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>693246</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>44207</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>25480725</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>8987322</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>4239775</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>8987322</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>8987322</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>937028</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>44208</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>27696150</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>9327138</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>4385175</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>9327138</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>9327138</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>951774</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>44209</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>29380125</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>10278462</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>4556575</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>10278462</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>10278462</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>1084177</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12">
+      <c r="A12" s="2" t="n">
         <v>44210</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>30628175</v>
       </c>
-      <c r="C12">
-        <f>F12-G12</f>
+      <c r="C12" t="n">
         <v>8348671</v>
       </c>
-      <c r="E12">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
         <v>11148991</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>9690757</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>1342086</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>1225493</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>44211</v>
+      </c>
+      <c r="B13" t="n">
+        <v>31161075</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>12279180</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10595866</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1610524</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1384963</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>44215</v>
+      </c>
+      <c r="B14" t="n">
+        <v>31161075</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>15707588</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13595803</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2023124</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1745441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New data and fixed date comprehension
</commit_message>
<xml_diff>
--- a/vaccine_data.xlsx
+++ b/vaccine_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -831,6 +831,50 @@
         <v>1908256</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>44217</v>
+      </c>
+      <c r="B16" t="n">
+        <v>37960000</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>17546374</v>
+      </c>
+      <c r="F16" t="n">
+        <v>15053257</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2394961</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2089181</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>44220</v>
+      </c>
+      <c r="B17" t="n">
+        <v>41411550</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>21848655</v>
+      </c>
+      <c r="F17" t="n">
+        <v>18502131</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3216836</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2567018</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>